<commit_message>
A days' work --> Procrastrination
</commit_message>
<xml_diff>
--- a/Grafer/Rådata för grafer.xlsx
+++ b/Grafer/Rådata för grafer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Agfa Healthcare</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Övriga</t>
+  </si>
+  <si>
+    <t>Totalt</t>
   </si>
 </sst>
 </file>
@@ -2501,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2602,6 +2605,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
commit for commits sake
</commit_message>
<xml_diff>
--- a/Grafer/Rådata för grafer.xlsx
+++ b/Grafer/Rådata för grafer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="646" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rådata för brancher" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Agfa Healthcare</t>
   </si>
@@ -235,6 +235,9 @@
   <si>
     <t>Large Scale Scrum: (Hela världen)</t>
   </si>
+  <si>
+    <t>RAGE</t>
+  </si>
 </sst>
 </file>
 
@@ -292,12 +295,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9740,9 +9744,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>VersionOne!$A$1:$A$9</c:f>
+              <c:f>VersionOne!$A$1:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Scrum of Scums</c:v>
                 </c:pt>
@@ -9769,16 +9773,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>DAD</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>RAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>VersionOne!$B$1:$B$9</c:f>
+              <c:f>VersionOne!$B$1:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.72</c:v>
                 </c:pt>
@@ -9804,7 +9811,10 @@
                   <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.05</c:v>
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17284,7 +17294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -20190,10 +20200,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20270,7 +20280,15 @@
         <v>49</v>
       </c>
       <c r="B9" s="2">
-        <v>0.05</v>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>